<commit_message>
lots more work done
</commit_message>
<xml_diff>
--- a/Lit Review/Charts and tables.xlsx
+++ b/Lit Review/Charts and tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamg\Desktop\Personal\PhD Research\PhD Research\PhD\Lit Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B88370-A109-4970-AF23-C577C446E0B3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ED8A6D-2322-4CCC-B3BF-123C6F07276A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{B6E10DF4-6656-4D52-944F-27D43DBE1C11}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>Stroke occurs</t>
   </si>
   <si>
-    <t>Consequences of ischema most prominent</t>
-  </si>
-  <si>
     <t>Secondary Effects reach full force</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>Dynamism Ends</t>
+  </si>
+  <si>
+    <t>Consequences of ischemia most prominent</t>
   </si>
 </sst>
 </file>
@@ -404,56 +404,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,7 +772,7 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,102 +785,102 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="17" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="19"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="16"/>
+      <c r="C5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="20"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
-      <c r="C5" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="12"/>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="20" t="s">
-        <v>21</v>
+      <c r="F7" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>22</v>
+        <v>12</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did a bit of work eh
</commit_message>
<xml_diff>
--- a/Lit Review/Charts and tables.xlsx
+++ b/Lit Review/Charts and tables.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamg\Desktop\Personal\PhD Research\PhD Research\PhD\Lit Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ED8A6D-2322-4CCC-B3BF-123C6F07276A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1D5712-EFB7-4284-A21D-601764EE56B9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{B6E10DF4-6656-4D52-944F-27D43DBE1C11}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" activeTab="1" xr2:uid="{B6E10DF4-6656-4D52-944F-27D43DBE1C11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Onset</t>
   </si>
@@ -100,13 +101,43 @@
   </si>
   <si>
     <t>Consequences of ischemia most prominent</t>
+  </si>
+  <si>
+    <t>Admittance Control</t>
+  </si>
+  <si>
+    <t>Impedance Control</t>
+  </si>
+  <si>
+    <t>Advantages</t>
+  </si>
+  <si>
+    <t>Disadvantages</t>
+  </si>
+  <si>
+    <t>Only requires a force sensor at the end effector</t>
+  </si>
+  <si>
+    <t>Lends itself to direct drive electric motors, which are more easy to move by torque control</t>
+  </si>
+  <si>
+    <t>Requires a robust position control inner loop</t>
+  </si>
+  <si>
+    <t>Does not require an accurate dynamic model</t>
+  </si>
+  <si>
+    <t>Requires an accurate dynamic model to ensure controller stability</t>
+  </si>
+  <si>
+    <t>Requires force sensors at each joint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +148,23 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -137,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -386,11 +434,194 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -454,6 +685,71 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -771,7 +1067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED1F485-6FB2-4718-8DA3-CB51B597E04B}">
   <dimension ref="B1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -894,4 +1190,159 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7303F0F1-A0B8-4B89-9AE3-B92A7F97463A}">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32"/>
+      <c r="B1" s="32"/>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="22"/>
+      <c r="C2" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+      <c r="B3" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="35"/>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="41"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="44"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G4:J4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>